<commit_message>
expanded db with general parameters
</commit_message>
<xml_diff>
--- a/findings/google_form_pure.xlsx
+++ b/findings/google_form_pure.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Work\db\eyetoai\findings\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="1872" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993"/>
   </bookViews>
   <sheets>
-    <sheet name="Form Responses 1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -20,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -35,11 +40,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Responder updated this value.</t>
+          <t>Responder updated this value.</t>
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0">
+    <comment ref="G7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,11 +54,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Responder updated this value.</t>
+          <t>Responder updated this value.</t>
         </r>
       </text>
     </comment>
-    <comment ref="I18" authorId="0">
+    <comment ref="BB7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -63,11 +68,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Responder updated this value.</t>
+          <t>Responder updated this value.</t>
         </r>
       </text>
     </comment>
-    <comment ref="BB7" authorId="0">
+    <comment ref="CU7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,11 +82,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Responder updated this value.</t>
+          <t>Responder updated this value.</t>
         </r>
       </text>
     </comment>
-    <comment ref="CU7" authorId="0">
+    <comment ref="I18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +96,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Responder updated this value.</t>
+          <t>Responder updated this value.</t>
         </r>
       </text>
     </comment>
@@ -102,982 +107,966 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="313">
   <si>
-    <t xml:space="preserve">Timestamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relevant Modality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Typical age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prevalence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Risk factors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional features</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of finding Mammography</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass shape [Oval]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass shape [Round]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass shape [Irregular]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass margin [Circumscribed]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass margin [Obscured]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass margin [Microlobulated]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass margin [Indistinct]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass margin [Spiculated]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass density Mammography  [High density]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass density Mammography  [Equal density]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass density Mammography  [Low density]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass density Mammography  [Fat-containing]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications - Typically benign [Skin]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications - Typically benign [Vascular]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications - Typically benign [Coarse or “popcorn-like”]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications - Typically benign [Large rod-like]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications - Typically benign [Round]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications - Typically benign [Rim]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications - Typically benign [Dystrophic]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications - Typically benign [Milk of calcium]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications - Typically benign [Suture]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications - Suspicious morphology [Amorphous]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications - Suspicious morphology [Coarse heterogeneous]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications - Suspicious morphology [Fine pleomorphic]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications - Suspicious morphology [Fine linear or fine-linear branching]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications - Distribution [Diffuse]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications - Distribution [Regional]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications - Distribution [Grouped]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications - Distribution [Linear]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications - Distribution [Segmental]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asymmetries [Asymmetry]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asymmetries [Global asymmetry]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asymmetries [Focal asymmetry]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asymmetries [Developing asymmetry]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lymph nodes [Lymph nodes – intramammary]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lymph nodes [Lymph nodes – axillary]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional findings [Architectural distortion]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional findings [Skin retraction]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional findings [Nipple retraction]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional findings [Skin thickening]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional findings [Trabecular thickening]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional findings [Solitary dilated duct]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of finding US</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass margin [Not circumscribed]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass margin [Indistinct (Not circumscribed)]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass margin [Angular (Not circumscribed)]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass margin [Microlobulated (Not circumscribed)]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass margin [Spiculated (Not circumscribed)]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Echo pattern [Anechoic]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Echo pattern [Hyperechoic]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Echo pattern [Complex cystic and solid]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Echo pattern [Hypoechoic]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Echo pattern [Isoechoic]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Echo pattern [Heterogeneous]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Posterior features [No posterior features]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Posterior features [Enhancement]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Posterior features [Shadowing]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Posterior features [Combined pattern]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications US [Calcifications in a mass]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications US [Calcifications outside of a mass]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcifications US [Intraductal calcifications]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional findings [Edema]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional findings [Vascularity: Absent]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional findings [Vascularity: Internal vascularity]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional findings [Vascularity: Vessels in rim]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional findings [Elasticity:  Soft]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional findings [Elasticity:  Intermediate]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional findings [Elasticity:  Hard]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Special cases [Simple cyst]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Special cases [Clustered microcysts]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Special cases [Complicated cyst]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Special cases [Mass in or on skin]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Special cases [Foreign body including implants]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Special cases [Vascular: AVMs]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Special cases [Vascular: Mondor disease]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Special cases [Postsurgical fluid collection]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Special cases [Fat necrosis]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of finding MRI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass margin [Irregular (Not circumscribed)]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass - Internal enhacement [Homogeneous Medium]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass - Internal enhacement [Heterogeneous Fast]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass - Internal enhacement [Rim enhancement Delayed phase Persistent]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass - Internal enhacement [Dark internal septations]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MRI features [T1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MRI features [T2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MRI features [T1+C]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kinetic curve assessment (Signal intensity(SI)/time curve description) [Initial phase: Slow]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kinetic curve assessment (Signal intensity(SI)/time curve description) [Initial phase: Medium]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kinetic curve assessment (Signal intensity(SI)/time curve description) [Initial phase: Fast]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kinetic curve assessment (Signal intensity(SI)/time curve description) [Delayed phase: Persistent]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kinetic curve assessment (Signal intensity(SI)/time curve description) [Delayed phase: Plateau]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kinetic curve assessment (Signal intensity(SI)/time curve description) [Delayed phase: Washout]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enhancement curve type - old</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-mass enhancement (NME) - Distribution [Focal]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-mass enhancement (NME) - Distribution [Linear]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-mass enhancement (NME) - Distribution [Segmental]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-mass enhancement (NME) - Distribution [Regional]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-mass enhancement (NME) - Distribution [Multiple regions]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-mass enhancement (NME) - Distribution [Diffuse]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-mass enhancement (NME) - Internal enhancement patterns [Homogeneous]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-mass enhancement (NME) - Internal enhancement patterns [Heterogeneous]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-mass enhancement (NME) - Internal enhancement patterns [Clumped]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-mass enhancement (NME) - Internal enhancement patterns [Clustered ring]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-enhancing findings [Ductal precontrast high signal on T1W]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-enhancing findings [Cyst]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-enhancing findings [Postoperative collections (hematoma/seroma)]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-enhancing findings [Post-therapy skin thickening and trabecular thickening]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-enhancing findings [Non-enhancing mass]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-enhancing findings [Architectural distortion]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-enhancing findings [Signal void from foreign bodies, clips, etc]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fat containing lesions [Lymph nodes – Normal]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fat containing lesions [Lymph nodes – Abnormal]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fat containing lesions [Fat necrosis]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fat containing lesions [Hamartoma]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fat containing lesions [Postoperative seroma/hematoma with fat]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional findings [Skin invasion: Direct invasion]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional findings [Skin invasion: Inflammatory cancer]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional findings [Pectoralis muscle invasion]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional findings [Chest wall invasion]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bi-Rads [0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bi-Rads [1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bi-Rads [2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bi-Rads [3]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bi-Rads [4]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bi-Rads [5]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bi-Rads [6]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Associated Conditions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Associated Diseases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Differential diagnosis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique finding 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique finding 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique finding 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique finding 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique finding 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique finding 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of unique findings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Orientation [Parallel]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Orientation [Not parallel]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass elasticity (Elastography) [Elasticity:  Soft]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass elasticity (Elastography) [Elasticity:  Intermediate]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass elasticity (Elastography) [Elasticity:  Hard]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Name of condition</t>
+  </si>
+  <si>
+    <t>Condition description</t>
+  </si>
+  <si>
+    <t>Data source</t>
+  </si>
+  <si>
+    <t>Relevant Modality</t>
+  </si>
+  <si>
+    <t>Typical age</t>
+  </si>
+  <si>
+    <t>Prevalence</t>
+  </si>
+  <si>
+    <t>Risk factors</t>
+  </si>
+  <si>
+    <t>Additional features</t>
+  </si>
+  <si>
+    <t>Type of finding Mammography</t>
+  </si>
+  <si>
+    <t>Mass shape [Oval]</t>
+  </si>
+  <si>
+    <t>Mass shape [Round]</t>
+  </si>
+  <si>
+    <t>Mass shape [Irregular]</t>
+  </si>
+  <si>
+    <t>Mass margin [Circumscribed]</t>
+  </si>
+  <si>
+    <t>Mass margin [Obscured]</t>
+  </si>
+  <si>
+    <t>Mass margin [Microlobulated]</t>
+  </si>
+  <si>
+    <t>Mass margin [Indistinct]</t>
+  </si>
+  <si>
+    <t>Mass margin [Spiculated]</t>
+  </si>
+  <si>
+    <t>Mass density Mammography  [High density]</t>
+  </si>
+  <si>
+    <t>Mass density Mammography  [Equal density]</t>
+  </si>
+  <si>
+    <t>Mass density Mammography  [Low density]</t>
+  </si>
+  <si>
+    <t>Mass density Mammography  [Fat-containing]</t>
+  </si>
+  <si>
+    <t>Calcifications - Typically benign [Skin]</t>
+  </si>
+  <si>
+    <t>Calcifications - Typically benign [Vascular]</t>
+  </si>
+  <si>
+    <t>Calcifications - Typically benign [Coarse or “popcorn-like”]</t>
+  </si>
+  <si>
+    <t>Calcifications - Typically benign [Large rod-like]</t>
+  </si>
+  <si>
+    <t>Calcifications - Typically benign [Round]</t>
+  </si>
+  <si>
+    <t>Calcifications - Typically benign [Rim]</t>
+  </si>
+  <si>
+    <t>Calcifications - Typically benign [Dystrophic]</t>
+  </si>
+  <si>
+    <t>Calcifications - Typically benign [Milk of calcium]</t>
+  </si>
+  <si>
+    <t>Calcifications - Typically benign [Suture]</t>
+  </si>
+  <si>
+    <t>Calcifications - Suspicious morphology [Amorphous]</t>
+  </si>
+  <si>
+    <t>Calcifications - Suspicious morphology [Coarse heterogeneous]</t>
+  </si>
+  <si>
+    <t>Calcifications - Suspicious morphology [Fine pleomorphic]</t>
+  </si>
+  <si>
+    <t>Calcifications - Suspicious morphology [Fine linear or fine-linear branching]</t>
+  </si>
+  <si>
+    <t>Calcifications - Distribution [Diffuse]</t>
+  </si>
+  <si>
+    <t>Calcifications - Distribution [Regional]</t>
+  </si>
+  <si>
+    <t>Calcifications - Distribution [Grouped]</t>
+  </si>
+  <si>
+    <t>Calcifications - Distribution [Linear]</t>
+  </si>
+  <si>
+    <t>Calcifications - Distribution [Segmental]</t>
+  </si>
+  <si>
+    <t>Asymmetries [Asymmetry]</t>
+  </si>
+  <si>
+    <t>Asymmetries [Global asymmetry]</t>
+  </si>
+  <si>
+    <t>Asymmetries [Focal asymmetry]</t>
+  </si>
+  <si>
+    <t>Asymmetries [Developing asymmetry]</t>
+  </si>
+  <si>
+    <t>Lymph nodes [Lymph nodes – intramammary]</t>
+  </si>
+  <si>
+    <t>Lymph nodes [Lymph nodes – axillary]</t>
+  </si>
+  <si>
+    <t>Additional findings [Architectural distortion]</t>
+  </si>
+  <si>
+    <t>Additional findings [Skin retraction]</t>
+  </si>
+  <si>
+    <t>Additional findings [Nipple retraction]</t>
+  </si>
+  <si>
+    <t>Additional findings [Skin thickening]</t>
+  </si>
+  <si>
+    <t>Additional findings [Trabecular thickening]</t>
+  </si>
+  <si>
+    <t>Additional findings [Solitary dilated duct]</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Type of finding US</t>
+  </si>
+  <si>
+    <t>Mass margin [Not circumscribed]</t>
+  </si>
+  <si>
+    <t>Mass margin [Indistinct (Not circumscribed)]</t>
+  </si>
+  <si>
+    <t>Mass margin [Angular (Not circumscribed)]</t>
+  </si>
+  <si>
+    <t>Mass margin [Microlobulated (Not circumscribed)]</t>
+  </si>
+  <si>
+    <t>Mass margin [Spiculated (Not circumscribed)]</t>
+  </si>
+  <si>
+    <t>Mass Echo pattern [Anechoic]</t>
+  </si>
+  <si>
+    <t>Mass Echo pattern [Hyperechoic]</t>
+  </si>
+  <si>
+    <t>Mass Echo pattern [Complex cystic and solid]</t>
+  </si>
+  <si>
+    <t>Mass Echo pattern [Hypoechoic]</t>
+  </si>
+  <si>
+    <t>Mass Echo pattern [Isoechoic]</t>
+  </si>
+  <si>
+    <t>Mass Echo pattern [Heterogeneous]</t>
+  </si>
+  <si>
+    <t>Mass Posterior features [No posterior features]</t>
+  </si>
+  <si>
+    <t>Mass Posterior features [Enhancement]</t>
+  </si>
+  <si>
+    <t>Mass Posterior features [Shadowing]</t>
+  </si>
+  <si>
+    <t>Mass Posterior features [Combined pattern]</t>
+  </si>
+  <si>
+    <t>Calcifications US [Calcifications in a mass]</t>
+  </si>
+  <si>
+    <t>Calcifications US [Calcifications outside of a mass]</t>
+  </si>
+  <si>
+    <t>Calcifications US [Intraductal calcifications]</t>
+  </si>
+  <si>
+    <t>Additional findings [Edema]</t>
+  </si>
+  <si>
+    <t>Additional findings [Vascularity: Absent]</t>
+  </si>
+  <si>
+    <t>Additional findings [Vascularity: Internal vascularity]</t>
+  </si>
+  <si>
+    <t>Additional findings [Vascularity: Vessels in rim]</t>
+  </si>
+  <si>
+    <t>Additional findings [Elasticity:  Soft]</t>
+  </si>
+  <si>
+    <t>Additional findings [Elasticity:  Intermediate]</t>
+  </si>
+  <si>
+    <t>Additional findings [Elasticity:  Hard]</t>
+  </si>
+  <si>
+    <t>Special cases [Simple cyst]</t>
+  </si>
+  <si>
+    <t>Special cases [Clustered microcysts]</t>
+  </si>
+  <si>
+    <t>Special cases [Complicated cyst]</t>
+  </si>
+  <si>
+    <t>Special cases [Mass in or on skin]</t>
+  </si>
+  <si>
+    <t>Special cases [Foreign body including implants]</t>
+  </si>
+  <si>
+    <t>Special cases [Vascular: AVMs]</t>
+  </si>
+  <si>
+    <t>Special cases [Vascular: Mondor disease]</t>
+  </si>
+  <si>
+    <t>Special cases [Postsurgical fluid collection]</t>
+  </si>
+  <si>
+    <t>Special cases [Fat necrosis]</t>
+  </si>
+  <si>
+    <t>Type of finding MRI</t>
+  </si>
+  <si>
+    <t>Mass margin [Irregular (Not circumscribed)]</t>
+  </si>
+  <si>
+    <t>Mass - Internal enhacement [Homogeneous Medium]</t>
+  </si>
+  <si>
+    <t>Mass - Internal enhacement [Heterogeneous Fast]</t>
+  </si>
+  <si>
+    <t>Mass - Internal enhacement [Rim enhancement Delayed phase Persistent]</t>
+  </si>
+  <si>
+    <t>Mass - Internal enhacement [Dark internal septations]</t>
+  </si>
+  <si>
+    <t>MRI features [T1]</t>
+  </si>
+  <si>
+    <t>MRI features [T2]</t>
+  </si>
+  <si>
+    <t>MRI features [T1+C]</t>
+  </si>
+  <si>
+    <t>Kinetic curve assessment (Signal intensity(SI)/time curve description) [Initial phase: Slow]</t>
+  </si>
+  <si>
+    <t>Kinetic curve assessment (Signal intensity(SI)/time curve description) [Initial phase: Medium]</t>
+  </si>
+  <si>
+    <t>Kinetic curve assessment (Signal intensity(SI)/time curve description) [Initial phase: Fast]</t>
+  </si>
+  <si>
+    <t>Kinetic curve assessment (Signal intensity(SI)/time curve description) [Delayed phase: Persistent]</t>
+  </si>
+  <si>
+    <t>Kinetic curve assessment (Signal intensity(SI)/time curve description) [Delayed phase: Plateau]</t>
+  </si>
+  <si>
+    <t>Kinetic curve assessment (Signal intensity(SI)/time curve description) [Delayed phase: Washout]</t>
+  </si>
+  <si>
+    <t>Enhancement curve type - old</t>
+  </si>
+  <si>
+    <t>Non-mass enhancement (NME) - Distribution [Focal]</t>
+  </si>
+  <si>
+    <t>Non-mass enhancement (NME) - Distribution [Linear]</t>
+  </si>
+  <si>
+    <t>Non-mass enhancement (NME) - Distribution [Segmental]</t>
+  </si>
+  <si>
+    <t>Non-mass enhancement (NME) - Distribution [Regional]</t>
+  </si>
+  <si>
+    <t>Non-mass enhancement (NME) - Distribution [Multiple regions]</t>
+  </si>
+  <si>
+    <t>Non-mass enhancement (NME) - Distribution [Diffuse]</t>
+  </si>
+  <si>
+    <t>Non-mass enhancement (NME) - Internal enhancement patterns [Homogeneous]</t>
+  </si>
+  <si>
+    <t>Non-mass enhancement (NME) - Internal enhancement patterns [Heterogeneous]</t>
+  </si>
+  <si>
+    <t>Non-mass enhancement (NME) - Internal enhancement patterns [Clumped]</t>
+  </si>
+  <si>
+    <t>Non-mass enhancement (NME) - Internal enhancement patterns [Clustered ring]</t>
+  </si>
+  <si>
+    <t>Non-enhancing findings [Ductal precontrast high signal on T1W]</t>
+  </si>
+  <si>
+    <t>Non-enhancing findings [Cyst]</t>
+  </si>
+  <si>
+    <t>Non-enhancing findings [Postoperative collections (hematoma/seroma)]</t>
+  </si>
+  <si>
+    <t>Non-enhancing findings [Post-therapy skin thickening and trabecular thickening]</t>
+  </si>
+  <si>
+    <t>Non-enhancing findings [Non-enhancing mass]</t>
+  </si>
+  <si>
+    <t>Non-enhancing findings [Architectural distortion]</t>
+  </si>
+  <si>
+    <t>Non-enhancing findings [Signal void from foreign bodies, clips, etc]</t>
+  </si>
+  <si>
+    <t>Fat containing lesions [Lymph nodes – Normal]</t>
+  </si>
+  <si>
+    <t>Fat containing lesions [Lymph nodes – Abnormal]</t>
+  </si>
+  <si>
+    <t>Fat containing lesions [Fat necrosis]</t>
+  </si>
+  <si>
+    <t>Fat containing lesions [Hamartoma]</t>
+  </si>
+  <si>
+    <t>Fat containing lesions [Postoperative seroma/hematoma with fat]</t>
+  </si>
+  <si>
+    <t>Additional findings [Skin invasion: Direct invasion]</t>
+  </si>
+  <si>
+    <t>Additional findings [Skin invasion: Inflammatory cancer]</t>
+  </si>
+  <si>
+    <t>Additional findings [Pectoralis muscle invasion]</t>
+  </si>
+  <si>
+    <t>Additional findings [Chest wall invasion]</t>
+  </si>
+  <si>
+    <t>Bi-Rads [0]</t>
+  </si>
+  <si>
+    <t>Bi-Rads [1]</t>
+  </si>
+  <si>
+    <t>Bi-Rads [2]</t>
+  </si>
+  <si>
+    <t>Bi-Rads [3]</t>
+  </si>
+  <si>
+    <t>Bi-Rads [4]</t>
+  </si>
+  <si>
+    <t>Bi-Rads [5]</t>
+  </si>
+  <si>
+    <t>Bi-Rads [6]</t>
+  </si>
+  <si>
+    <t>Associated Conditions</t>
+  </si>
+  <si>
+    <t>Associated Diseases</t>
+  </si>
+  <si>
+    <t>Differential diagnosis</t>
+  </si>
+  <si>
+    <t>Unique finding 1</t>
+  </si>
+  <si>
+    <t>Unique finding 2</t>
+  </si>
+  <si>
+    <t>Unique finding 3</t>
+  </si>
+  <si>
+    <t>Unique finding 4</t>
+  </si>
+  <si>
+    <t>Unique finding 5</t>
+  </si>
+  <si>
+    <t>Unique finding 6</t>
+  </si>
+  <si>
+    <t>Number of unique findings</t>
+  </si>
+  <si>
+    <t>Mass Orientation [Parallel]</t>
+  </si>
+  <si>
+    <t>Mass Orientation [Not parallel]</t>
+  </si>
+  <si>
+    <t>Mass elasticity (Elastography) [Elasticity:  Soft]</t>
+  </si>
+  <si>
+    <t>Mass elasticity (Elastography) [Elasticity:  Intermediate]</t>
+  </si>
+  <si>
+    <t>Mass elasticity (Elastography) [Elasticity:  Hard]</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
   <si>
     <t xml:space="preserve">Purpose </t>
   </si>
   <si>
-    <t xml:space="preserve">Additional condition names</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enhancement curve type [type I curve: progressive enhancement pattern]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enhancement curve type [type II curve: plateau pattern]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enhancement curve type [type III curve: washout pattern]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass elasticity (elastography) [Elasticity:  Hard]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass elasticity (elastography) [Elasticity:  Soft]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass elasticity (elastography) [Elasticity:  Intermediate]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Orientation [Not circumscribed]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Orientation [Indistinct (Not circumscribed)]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Orientation [Angular (Not circumscribed)]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Orientation [Microlobulated (Not circumscribed)]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Orientation [Spiculated (Not circumscribed)]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fibroadenoma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fibroadenomas are the most common cause of a benign solid mass in the breast.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G&amp;E , Radiopaedia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mammography, US, MRI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">most common cause of a benign solid mass in the breast.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cyclosporin use</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Typical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atypical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Possible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unrelated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass, Calcification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Negative</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hyperechogenicity compared with fat, an oval or well-circumscribed lobulated or gently curving shape and the presence of a thin echogenic pseudocapsule. If these features are present with no features suggestive of malignancy, then a mass can be confidently classified as benign.
+    <t>Additional condition names</t>
+  </si>
+  <si>
+    <t>Enhancement curve type [type I curve: progressive enhancement pattern]</t>
+  </si>
+  <si>
+    <t>Enhancement curve type [type II curve: plateau pattern]</t>
+  </si>
+  <si>
+    <t>Enhancement curve type [type III curve: washout pattern]</t>
+  </si>
+  <si>
+    <t>Mass elasticity (elastography) [Elasticity:  Hard]</t>
+  </si>
+  <si>
+    <t>Mass elasticity (elastography) [Elasticity:  Soft]</t>
+  </si>
+  <si>
+    <t>Mass elasticity (elastography) [Elasticity:  Intermediate]</t>
+  </si>
+  <si>
+    <t>Mass Orientation [Not circumscribed]</t>
+  </si>
+  <si>
+    <t>Mass Orientation [Indistinct (Not circumscribed)]</t>
+  </si>
+  <si>
+    <t>Mass Orientation [Angular (Not circumscribed)]</t>
+  </si>
+  <si>
+    <t>Mass Orientation [Microlobulated (Not circumscribed)]</t>
+  </si>
+  <si>
+    <t>Mass Orientation [Spiculated (Not circumscribed)]</t>
+  </si>
+  <si>
+    <t>Fibroadenoma</t>
+  </si>
+  <si>
+    <t>Fibroadenomas are the most common cause of a benign solid mass in the breast.</t>
+  </si>
+  <si>
+    <t>G&amp;E , Radiopaedia</t>
+  </si>
+  <si>
+    <t>Mammography, US, MRI</t>
+  </si>
+  <si>
+    <t>20-30</t>
+  </si>
+  <si>
+    <t>most common cause of a benign solid mass in the breast.</t>
+  </si>
+  <si>
+    <t>cyclosporin use</t>
+  </si>
+  <si>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>Typical</t>
+  </si>
+  <si>
+    <t>Atypical</t>
+  </si>
+  <si>
+    <t>Possible</t>
+  </si>
+  <si>
+    <t>Unrelated</t>
+  </si>
+  <si>
+    <t>Mass, Calcification</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>hyperechogenicity compared with fat, an oval or well-circumscribed lobulated or gently curving shape and the presence of a thin echogenic pseudocapsule. If these features are present with no features suggestive of malignancy, then a mass can be confidently classified as benign.
 Most fibroadenomas are isoechoic or mildly hypoechoic relative to fat, with an oval shape and lobulated contour. A thin echogenic pseudocapsule may be seen.</t>
   </si>
   <si>
-    <t xml:space="preserve">Cowden syndrome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Breast Ca.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Papilloma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Papillomas are benign neoplasms, arising in a duct, either centrally or peripherally within the breast. Many papillomas secrete watery material, leading to a nipple discharge. As they are often friable and bleed easily, the discharge may be bloodstained.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G&amp;E, Radiopaedia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40-50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass, Calcification, Asymmetries, Additional findings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mammography
+    <t>Cowden syndrome</t>
+  </si>
+  <si>
+    <t>Breast Ca.</t>
+  </si>
+  <si>
+    <t>Papilloma</t>
+  </si>
+  <si>
+    <t>Papillomas are benign neoplasms, arising in a duct, either centrally or peripherally within the breast. Many papillomas secrete watery material, leading to a nipple discharge. As they are often friable and bleed easily, the discharge may be bloodstained.</t>
+  </si>
+  <si>
+    <t>G&amp;E, Radiopaedia</t>
+  </si>
+  <si>
+    <t>40-50</t>
+  </si>
+  <si>
+    <t>Mass, Calcification, Asymmetries, Additional findings</t>
+  </si>
+  <si>
+    <t>Mammography
 Mammograms are frequently normal (particularly with small intraductal papillomas). When imaging findings are present, they include solitary or multiple dilated ducts, a circumscribed benign-appearing mass (often subareolar in location), or a cluster of calcifications.</t>
   </si>
   <si>
-    <t xml:space="preserve">ductal carcinoma in situ (DCIS)
+    <t>ductal carcinoma in situ (DCIS)
 invasive ductal carcinoma with an in situ component
 papillary carcinoma of the breast can mimic an intraductal papilloma (particularly on ultrasound)</t>
   </si>
   <si>
-    <t xml:space="preserve">Condition 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Book</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mammography</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-10, 30-40, 60-70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3, 4, 5vtg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invasive ductal carcinoma (IDC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">breast cancer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B.A. Shah et al., Breast Imaging Review: A Quick Guide to Essential Diagnoses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mammography, US</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass, Additional findings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mastitis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">breast inflammation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asymmetries, Additional findings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional findings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">increased echogenicity of
+    <t>Condition 1</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Book</t>
+  </si>
+  <si>
+    <t>Mammography</t>
+  </si>
+  <si>
+    <t>0-10, 30-40, 60-70</t>
+  </si>
+  <si>
+    <t>3, 4, 5vtg</t>
+  </si>
+  <si>
+    <t>Invasive ductal carcinoma (IDC)</t>
+  </si>
+  <si>
+    <t>breast cancer</t>
+  </si>
+  <si>
+    <t>B.A. Shah et al., Breast Imaging Review: A Quick Guide to Essential Diagnoses</t>
+  </si>
+  <si>
+    <t>Mammography, US</t>
+  </si>
+  <si>
+    <t>Mass, Additional findings</t>
+  </si>
+  <si>
+    <t>Mastitis</t>
+  </si>
+  <si>
+    <t>breast inflammation</t>
+  </si>
+  <si>
+    <t>Asymmetries, Additional findings</t>
+  </si>
+  <si>
+    <t>Additional findings</t>
+  </si>
+  <si>
+    <t>increased echogenicity of
 the breast</t>
   </si>
   <si>
-    <t xml:space="preserve">Reactive lymphadenopathy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lymphoma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lymphoma accounts for approximately 0.1–0.2 % of all breast carcinomas, More commonly lymphoma occurs in the breast due to metastasis of extramammary lymphoma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-mass enhancement (NME)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type III curve: washout pattern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">primary breast lymphoma, extramammary lymphoma metastasis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FIBROADENOMA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fibroadenoma is a benign fi broepithelial tumor with
+    <t>Reactive lymphadenopathy</t>
+  </si>
+  <si>
+    <t>lymphoma</t>
+  </si>
+  <si>
+    <t>Lymphoma accounts for approximately 0.1–0.2 % of all breast carcinomas, More commonly lymphoma occurs in the breast due to metastasis of extramammary lymphoma</t>
+  </si>
+  <si>
+    <t>Non-mass enhancement (NME)</t>
+  </si>
+  <si>
+    <t>type III curve: washout pattern</t>
+  </si>
+  <si>
+    <t>primary breast lymphoma, extramammary lymphoma metastasis</t>
+  </si>
+  <si>
+    <t>FIBROADENOMA</t>
+  </si>
+  <si>
+    <t>Fibroadenoma is a benign fi broepithelial tumor with
 mixed stromal and epithelial elements</t>
   </si>
   <si>
-    <t xml:space="preserve">US</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIPOMA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A lipoma is a benign fatty mass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass, Architectural distortion, Additional findings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INVASIVE LOBULAR CARCINOMA (ILC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ILC arises from the lobular epithelium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It is the second most common breast cancer and accounts for 10–15 % of all invasive breast malignancies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ascites, pelvic masses, hydronephrosis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pet: high rate of false-negative findings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mammo: shrinking breast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sebaceous cysts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sebaceous cysts are retention cysts and are believed to arise from the acral surface of the skin by implantation of the epidermis into the dermis.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Breast Imaging: Expert Radiology Series</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US, MRI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sebaceous cysts are rare  within the breast parenchyma.\</t>
-  </si>
-  <si>
-    <t xml:space="preserve">carcinoma, fibroadenoma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skin: claw sign</t>
-  </si>
-  <si>
-    <t xml:space="preserve">muhammad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Galactocele</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A galactocele is a benign milk-filled cyst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Galactoceles almost always occur in women during or just after cessation of lactation and rarely occur in men, A galactocele is presumably caused by ductal obstruction.  It is not a common lesion but can be seen in pregnancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pregnancy, chronic galactorrhea, pituitary adenoma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hamartoma, lipoma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mammo: A circumscribed mass with a fat-fluid level on a mediolateral or lateromedial projection is diagnostic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">muhammmad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duct ectasia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duct ectasia is a nonspecific dilation of the major subareolar ducts, with occasional involvement of smaller ducts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duct ectasia has been found in women of all ages and is  rarely seen in men</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcification, Additional findings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ignore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plasma cell mastitis, obliterate mastitis, comedomastitis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">us: dilated ducts that may be filled with anechoic fluid, echogenic debris, or both</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epidermal inclusion cyst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epidermal inclusion cysts usually arise from obstruction of the infundibular portion of the hair follicle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epidermal inclusion cysts are not common in the breast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reduction mammoplasty, iatrogenic procedures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">infundibular cyst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fibrocystic breast changes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fibrocystic change is not a disease but refers to a constellation of benign histologic findings. It was previously referred to as fibrocystic disease, a name that should no longer be used because the symptoms are within
+    <t>US</t>
+  </si>
+  <si>
+    <t>LIPOMA</t>
+  </si>
+  <si>
+    <t>A lipoma is a benign fatty mass</t>
+  </si>
+  <si>
+    <t>Mass, Architectural distortion, Additional findings</t>
+  </si>
+  <si>
+    <t>INVASIVE LOBULAR CARCINOMA (ILC)</t>
+  </si>
+  <si>
+    <t>ILC arises from the lobular epithelium</t>
+  </si>
+  <si>
+    <t>It is the second most common breast cancer and accounts for 10–15 % of all invasive breast malignancies</t>
+  </si>
+  <si>
+    <t>ascites, pelvic masses, hydronephrosis</t>
+  </si>
+  <si>
+    <t>pet: high rate of false-negative findings</t>
+  </si>
+  <si>
+    <t>mammo: shrinking breast</t>
+  </si>
+  <si>
+    <t>Sebaceous cysts</t>
+  </si>
+  <si>
+    <t>Sebaceous cysts are retention cysts and are believed to arise from the acral surface of the skin by implantation of the epidermis into the dermis.</t>
+  </si>
+  <si>
+    <t>Breast Imaging: Expert Radiology Series</t>
+  </si>
+  <si>
+    <t>US, MRI</t>
+  </si>
+  <si>
+    <t>Sebaceous cysts are rare  within the breast parenchyma.\</t>
+  </si>
+  <si>
+    <t>carcinoma, fibroadenoma</t>
+  </si>
+  <si>
+    <t>skin: claw sign</t>
+  </si>
+  <si>
+    <t>muhammad</t>
+  </si>
+  <si>
+    <t>Galactocele</t>
+  </si>
+  <si>
+    <t>A galactocele is a benign milk-filled cyst</t>
+  </si>
+  <si>
+    <t>Galactoceles almost always occur in women during or just after cessation of lactation and rarely occur in men, A galactocele is presumably caused by ductal obstruction.  It is not a common lesion but can be seen in pregnancy</t>
+  </si>
+  <si>
+    <t>pregnancy, chronic galactorrhea, pituitary adenoma</t>
+  </si>
+  <si>
+    <t>hamartoma, lipoma</t>
+  </si>
+  <si>
+    <t>mammo: A circumscribed mass with a fat-fluid level on a mediolateral or lateromedial projection is diagnostic</t>
+  </si>
+  <si>
+    <t>muhammmad</t>
+  </si>
+  <si>
+    <t>Duct ectasia</t>
+  </si>
+  <si>
+    <t>Duct ectasia is a nonspecific dilation of the major subareolar ducts, with occasional involvement of smaller ducts</t>
+  </si>
+  <si>
+    <t>Duct ectasia has been found in women of all ages and is  rarely seen in men</t>
+  </si>
+  <si>
+    <t>Calcification, Additional findings</t>
+  </si>
+  <si>
+    <t>Ignore</t>
+  </si>
+  <si>
+    <t>plasma cell mastitis, obliterate mastitis, comedomastitis</t>
+  </si>
+  <si>
+    <t>us: dilated ducts that may be filled with anechoic fluid, echogenic debris, or both</t>
+  </si>
+  <si>
+    <t>Epidermal inclusion cyst</t>
+  </si>
+  <si>
+    <t>Epidermal inclusion cysts usually arise from obstruction of the infundibular portion of the hair follicle</t>
+  </si>
+  <si>
+    <t>Epidermal inclusion cysts are not common in the breast</t>
+  </si>
+  <si>
+    <t>reduction mammoplasty, iatrogenic procedures</t>
+  </si>
+  <si>
+    <t>infundibular cyst</t>
+  </si>
+  <si>
+    <t>Fibrocystic breast changes</t>
+  </si>
+  <si>
+    <t>Fibrocystic change is not a disease but refers to a constellation of benign histologic findings. It was previously referred to as fibrocystic disease, a name that should no longer be used because the symptoms are within
 the normal spectrum of hormone-related changes in the breast</t>
   </si>
   <si>
-    <t xml:space="preserve">Fibrocystic change is a common finding in younger and premenopausal women</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fibrocystic changes are known to be associated with hormonal shifts in estrogen and progesterone, which affectthe breast tissue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">normal breast tissue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fibrocystic disease</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mammo: normal breast tissue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fibroadenoma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A fibroadenoma is a benign fibroepithelial proliferative tumor with the hallmark of a concurrent proliferation of glandular and stromal elements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fibroadenomas are the most common breast masses encountered in women younger than 35 years of age and the most common solid masses found in women of all ages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">influenced by estrogen levels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass, Non-mass enhancement (NME)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Low</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intramammary lymph nodes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An intramammary lymph node is a lymph node found within the breast parenchyma at any quadrant excluding axillary lymph nodes, The vast majority seen on mammography are in the upper outer quadrant of the breast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lymph nodes are commonly encountered on mammograms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass, Fat containing lesions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hamartoma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hamartomas are benign well circumscribed breast lesions composed of variable normal constituents of breast tissue including fat, glandular tissue, and fibrous connective tissue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40-50, 50-60, 60-70, 70+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The majority of the hamartomas are detected in women  older than 35 years of age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cut sausage sign, breast within a breast sign</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mammo: thin radiopaque capsule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mri: thin radiopaque capsule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">us: thin radiopaque capsule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fibroadenolipoma, Lipofibroadenoma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lipoma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lipomas are benign fatty tumors that may occur anywhere within the breast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">movable. A lipoma is one of the more  common causes of a palpable finding in a male patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mammo: thin radiopaque capsule is classic.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fibromatosis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fibromatosis of the breast is a benign localized proliferation of fibroblasts that is nonmalignant but does have a tendency to recur after excision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30-40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fibromatosis usually occurs in the abdominal wall and superficial muscular-aponeurotic tissues of the extremities. Pathologic diagnosis of fibromatosis of the breast is  extremely rare, with an incidence as low as 0.2% of breast  tumors. It may arise from the pectoralis muscle/fascia or  mammary tissue as a primary tumor.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass, Calcification, Additional findings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type I curve: progressive enhancement pattern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">extra-abdominal desmoid tumor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fibrosis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fibrosis is a benign proliferation of fibrous connective tissue of the breast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">may represent as much as 2.1% to 9% of lesions found in patients who undergo image-guided core biopsy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">history of trauma with scar tissue, surgical history, history of insulin dependent diabetes mellitus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass, Architectural distortion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">focal fibrous disease of the breast, fibrosis of the breast, fibrous mastopathy, fibrous tumor of the breast, focal fibrosis of the breast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adenosis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adenosis is a spectrum of histologic lesions ranging from hyperplasia of the lobule to sclerosing adenosis with fibrosis and calcifications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">occurring during the reproductive years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lactating adenomas are often associated with pregnancy and puerperium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pregnancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tubular adenomas, lactating adenomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diabetic mastopathy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diabetic mastopathy is a condition in which stromal proliferation forms fibrous tumors predominately in patients with insulin-dependent diabetes mellitus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">histocompatibility locus antigen (HLA)-associated autoimmune diseases, insulin-dependent diabetes mellitus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass, Asymmetries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Granular cell tumor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Granular cell tumor is an uncommon usually benign tumor originating from Schwann cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5% to 6% of granular cell tumors occur in the breast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fat necrosis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fat necrosis involves necrosis of adipose tissue and is characterized by the formation of small quantities of calcium soaps when fat is hydrolyzed into glycerol and fatty acids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fat necrosis is a common benign condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trauma (including surgery)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass, Calcification, Architectural distortion</t>
+    <t>Fibrocystic change is a common finding in younger and premenopausal women</t>
+  </si>
+  <si>
+    <t>Fibrocystic changes are known to be associated with hormonal shifts in estrogen and progesterone, which affectthe breast tissue</t>
+  </si>
+  <si>
+    <t>normal breast tissue</t>
+  </si>
+  <si>
+    <t>fibrocystic disease</t>
+  </si>
+  <si>
+    <t>mammo: normal breast tissue</t>
+  </si>
+  <si>
+    <t>fibroadenoma</t>
+  </si>
+  <si>
+    <t>A fibroadenoma is a benign fibroepithelial proliferative tumor with the hallmark of a concurrent proliferation of glandular and stromal elements</t>
+  </si>
+  <si>
+    <t>Fibroadenomas are the most common breast masses encountered in women younger than 35 years of age and the most common solid masses found in women of all ages</t>
+  </si>
+  <si>
+    <t>influenced by estrogen levels</t>
+  </si>
+  <si>
+    <t>Mass, Non-mass enhancement (NME)</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Intramammary lymph nodes</t>
+  </si>
+  <si>
+    <t>An intramammary lymph node is a lymph node found within the breast parenchyma at any quadrant excluding axillary lymph nodes, The vast majority seen on mammography are in the upper outer quadrant of the breast</t>
+  </si>
+  <si>
+    <t>Lymph nodes are commonly encountered on mammograms</t>
+  </si>
+  <si>
+    <t>Mass, Fat containing lesions</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Hamartoma</t>
+  </si>
+  <si>
+    <t>Hamartomas are benign well circumscribed breast lesions composed of variable normal constituents of breast tissue including fat, glandular tissue, and fibrous connective tissue</t>
+  </si>
+  <si>
+    <t>40-50, 50-60, 60-70, 70+</t>
+  </si>
+  <si>
+    <t>The majority of the hamartomas are detected in women  older than 35 years of age</t>
+  </si>
+  <si>
+    <t>cut sausage sign, breast within a breast sign</t>
+  </si>
+  <si>
+    <t>mammo: thin radiopaque capsule</t>
+  </si>
+  <si>
+    <t>mri: thin radiopaque capsule</t>
+  </si>
+  <si>
+    <t>us: thin radiopaque capsule</t>
+  </si>
+  <si>
+    <t>Fibroadenolipoma, Lipofibroadenoma</t>
+  </si>
+  <si>
+    <t>Lipoma</t>
+  </si>
+  <si>
+    <t>Lipomas are benign fatty tumors that may occur anywhere within the breast</t>
+  </si>
+  <si>
+    <t>movable. A lipoma is one of the more  common causes of a palpable finding in a male patient</t>
+  </si>
+  <si>
+    <t>mammo: thin radiopaque capsule is classic.</t>
+  </si>
+  <si>
+    <t>Fibromatosis</t>
+  </si>
+  <si>
+    <t>Fibromatosis of the breast is a benign localized proliferation of fibroblasts that is nonmalignant but does have a tendency to recur after excision</t>
+  </si>
+  <si>
+    <t>30-40</t>
+  </si>
+  <si>
+    <t>Fibromatosis usually occurs in the abdominal wall and superficial muscular-aponeurotic tissues of the extremities. Pathologic diagnosis of fibromatosis of the breast is  extremely rare, with an incidence as low as 0.2% of breast  tumors. It may arise from the pectoralis muscle/fascia or  mammary tissue as a primary tumor.</t>
+  </si>
+  <si>
+    <t>Mass, Calcification, Additional findings</t>
+  </si>
+  <si>
+    <t>type I curve: progressive enhancement pattern</t>
+  </si>
+  <si>
+    <t>extra-abdominal desmoid tumor</t>
+  </si>
+  <si>
+    <t>Fibrosis</t>
+  </si>
+  <si>
+    <t>Fibrosis is a benign proliferation of fibrous connective tissue of the breast</t>
+  </si>
+  <si>
+    <t>may represent as much as 2.1% to 9% of lesions found in patients who undergo image-guided core biopsy</t>
+  </si>
+  <si>
+    <t>history of trauma with scar tissue, surgical history, history of insulin dependent diabetes mellitus</t>
+  </si>
+  <si>
+    <t>Mass, Architectural distortion</t>
+  </si>
+  <si>
+    <t>focal fibrous disease of the breast, fibrosis of the breast, fibrous mastopathy, fibrous tumor of the breast, focal fibrosis of the breast</t>
+  </si>
+  <si>
+    <t>Adenosis</t>
+  </si>
+  <si>
+    <t>Adenosis is a spectrum of histologic lesions ranging from hyperplasia of the lobule to sclerosing adenosis with fibrosis and calcifications</t>
+  </si>
+  <si>
+    <t>occurring during the reproductive years</t>
+  </si>
+  <si>
+    <t>Lactating adenomas are often associated with pregnancy and puerperium</t>
+  </si>
+  <si>
+    <t>pregnancy</t>
+  </si>
+  <si>
+    <t>tubular adenomas, lactating adenomas</t>
+  </si>
+  <si>
+    <t>Diabetic mastopathy</t>
+  </si>
+  <si>
+    <t>Diabetic mastopathy is a condition in which stromal proliferation forms fibrous tumors predominately in patients with insulin-dependent diabetes mellitus</t>
+  </si>
+  <si>
+    <t>histocompatibility locus antigen (HLA)-associated autoimmune diseases, insulin-dependent diabetes mellitus</t>
+  </si>
+  <si>
+    <t>Mass, Asymmetries</t>
+  </si>
+  <si>
+    <t>Granular cell tumor</t>
+  </si>
+  <si>
+    <t>Granular cell tumor is an uncommon usually benign tumor originating from Schwann cells</t>
+  </si>
+  <si>
+    <t>5% to 6% of granular cell tumors occur in the breast</t>
+  </si>
+  <si>
+    <t>Fat necrosis</t>
+  </si>
+  <si>
+    <t>Fat necrosis involves necrosis of adipose tissue and is characterized by the formation of small quantities of calcium soaps when fat is hydrolyzed into glycerol and fatty acids</t>
+  </si>
+  <si>
+    <t>Fat necrosis is a common benign condition</t>
+  </si>
+  <si>
+    <t>trauma (including surgery)</t>
+  </si>
+  <si>
+    <t>Mass, Calcification, Architectural distortion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="M/D/YYYY\ H:MM:SS"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1095,7 +1084,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1103,156 +1092,677 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1767840</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>259080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1034" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF2C7260-D16D-4131-8FAF-4312E58B58AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1767840</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>259080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1032" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEB8C7F2-B8A1-4401-BE88-2CD98E9EA958}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1767840</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>259080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1030" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2591A00C-0D7D-4FEC-A411-691DE340BAC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1767840</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>259080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D860CC3-5598-40E6-B97C-E856F210E066}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1767840</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>259080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D2A39AE-50B1-45B8-984F-546DDA569571}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:GU65536"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:GU1048575"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.8520408163265"/>
-    <col collapsed="false" hidden="false" max="9" min="6" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="58.9081632653061"/>
-    <col collapsed="false" hidden="false" max="52" min="11" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="68.4948979591837"/>
-    <col collapsed="false" hidden="false" max="71" min="54" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="72" min="72" style="0" width="33.4795918367347"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="74" min="74" style="0" width="23.6326530612245"/>
-    <col collapsed="false" hidden="false" max="79" min="75" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="80" min="80" style="0" width="50.2959183673469"/>
-    <col collapsed="false" hidden="false" max="203" min="81" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="204" style="0" width="14.1734693877551"/>
+    <col min="1" max="4" width="21.33203125"/>
+    <col min="5" max="5" width="45.88671875"/>
+    <col min="6" max="9" width="21.33203125"/>
+    <col min="10" max="10" width="58.88671875"/>
+    <col min="11" max="18" width="21.33203125"/>
+    <col min="19" max="19" width="39.33203125" customWidth="1"/>
+    <col min="20" max="20" width="46.33203125" customWidth="1"/>
+    <col min="21" max="21" width="46.5546875" customWidth="1"/>
+    <col min="22" max="23" width="21.33203125"/>
+    <col min="24" max="24" width="54.6640625" customWidth="1"/>
+    <col min="25" max="25" width="41.109375" customWidth="1"/>
+    <col min="26" max="52" width="21.33203125"/>
+    <col min="53" max="53" width="68.44140625"/>
+    <col min="54" max="71" width="21.33203125"/>
+    <col min="72" max="72" width="33.44140625"/>
+    <col min="73" max="73" width="21.33203125"/>
+    <col min="74" max="74" width="23.6640625"/>
+    <col min="75" max="79" width="21.33203125"/>
+    <col min="80" max="80" width="50.33203125"/>
+    <col min="81" max="203" width="21.33203125"/>
+    <col min="204" max="1025" width="14.21875"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:203" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" t="s">
         <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
@@ -1282,268 +1792,268 @@
       <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="0" t="s">
+      <c r="AF1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="0" t="s">
+      <c r="AG1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="0" t="s">
+      <c r="AH1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="0" t="s">
+      <c r="AI1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="0" t="s">
+      <c r="AJ1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="0" t="s">
+      <c r="AK1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="0" t="s">
+      <c r="AL1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="0" t="s">
+      <c r="AM1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="0" t="s">
+      <c r="AN1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="0" t="s">
+      <c r="AO1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="0" t="s">
+      <c r="AP1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="0" t="s">
+      <c r="AQ1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="0" t="s">
+      <c r="AR1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="0" t="s">
+      <c r="AS1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="0" t="s">
+      <c r="AT1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="0" t="s">
+      <c r="AU1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="0" t="s">
+      <c r="AV1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="0" t="s">
+      <c r="AW1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="0" t="s">
+      <c r="AX1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="0" t="s">
+      <c r="AY1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="0" t="s">
+      <c r="AZ1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="0" t="s">
+      <c r="BA1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="0" t="s">
+      <c r="BB1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="0" t="s">
+      <c r="BC1" t="s">
         <v>10</v>
       </c>
-      <c r="BD1" s="0" t="s">
+      <c r="BD1" t="s">
         <v>11</v>
       </c>
-      <c r="BE1" s="0" t="s">
+      <c r="BE1" t="s">
         <v>12</v>
       </c>
-      <c r="BF1" s="0" t="s">
+      <c r="BF1" t="s">
         <v>13</v>
       </c>
-      <c r="BG1" s="0" t="s">
+      <c r="BG1" t="s">
         <v>54</v>
       </c>
-      <c r="BH1" s="0" t="s">
+      <c r="BH1" t="s">
         <v>55</v>
       </c>
-      <c r="BI1" s="0" t="s">
+      <c r="BI1" t="s">
         <v>56</v>
       </c>
-      <c r="BJ1" s="0" t="s">
+      <c r="BJ1" t="s">
         <v>57</v>
       </c>
-      <c r="BK1" s="0" t="s">
+      <c r="BK1" t="s">
         <v>58</v>
       </c>
-      <c r="BL1" s="0" t="s">
+      <c r="BL1" t="s">
         <v>59</v>
       </c>
-      <c r="BM1" s="0" t="s">
+      <c r="BM1" t="s">
         <v>60</v>
       </c>
-      <c r="BN1" s="0" t="s">
+      <c r="BN1" t="s">
         <v>61</v>
       </c>
-      <c r="BO1" s="0" t="s">
+      <c r="BO1" t="s">
         <v>62</v>
       </c>
-      <c r="BP1" s="0" t="s">
+      <c r="BP1" t="s">
         <v>63</v>
       </c>
-      <c r="BQ1" s="0" t="s">
+      <c r="BQ1" t="s">
         <v>64</v>
       </c>
-      <c r="BR1" s="0" t="s">
+      <c r="BR1" t="s">
         <v>65</v>
       </c>
-      <c r="BS1" s="0" t="s">
+      <c r="BS1" t="s">
         <v>66</v>
       </c>
-      <c r="BT1" s="0" t="s">
+      <c r="BT1" t="s">
         <v>67</v>
       </c>
-      <c r="BU1" s="0" t="s">
+      <c r="BU1" t="s">
         <v>68</v>
       </c>
-      <c r="BV1" s="0" t="s">
+      <c r="BV1" t="s">
         <v>69</v>
       </c>
-      <c r="BW1" s="0" t="s">
+      <c r="BW1" t="s">
         <v>70</v>
       </c>
-      <c r="BX1" s="0" t="s">
+      <c r="BX1" t="s">
         <v>71</v>
       </c>
-      <c r="BY1" s="0" t="s">
+      <c r="BY1" t="s">
         <v>44</v>
       </c>
-      <c r="BZ1" s="0" t="s">
+      <c r="BZ1" t="s">
         <v>45</v>
       </c>
-      <c r="CA1" s="0" t="s">
+      <c r="CA1" t="s">
         <v>46</v>
       </c>
-      <c r="CB1" s="0" t="s">
+      <c r="CB1" t="s">
         <v>49</v>
       </c>
-      <c r="CC1" s="0" t="s">
+      <c r="CC1" t="s">
         <v>47</v>
       </c>
-      <c r="CD1" s="0" t="s">
+      <c r="CD1" t="s">
         <v>72</v>
       </c>
-      <c r="CE1" s="0" t="s">
+      <c r="CE1" t="s">
         <v>73</v>
       </c>
-      <c r="CF1" s="0" t="s">
+      <c r="CF1" t="s">
         <v>74</v>
       </c>
-      <c r="CG1" s="0" t="s">
+      <c r="CG1" t="s">
         <v>75</v>
       </c>
-      <c r="CH1" s="0" t="s">
+      <c r="CH1" t="s">
         <v>76</v>
       </c>
-      <c r="CI1" s="0" t="s">
+      <c r="CI1" t="s">
         <v>77</v>
       </c>
-      <c r="CJ1" s="0" t="s">
+      <c r="CJ1" t="s">
         <v>78</v>
       </c>
-      <c r="CK1" s="0" t="s">
+      <c r="CK1" t="s">
         <v>79</v>
       </c>
-      <c r="CL1" s="0" t="s">
+      <c r="CL1" t="s">
         <v>80</v>
       </c>
-      <c r="CM1" s="0" t="s">
+      <c r="CM1" t="s">
         <v>81</v>
       </c>
-      <c r="CN1" s="0" t="s">
+      <c r="CN1" t="s">
         <v>82</v>
       </c>
-      <c r="CO1" s="0" t="s">
+      <c r="CO1" t="s">
         <v>83</v>
       </c>
-      <c r="CP1" s="0" t="s">
+      <c r="CP1" t="s">
         <v>84</v>
       </c>
-      <c r="CQ1" s="0" t="s">
+      <c r="CQ1" t="s">
         <v>85</v>
       </c>
-      <c r="CR1" s="0" t="s">
+      <c r="CR1" t="s">
         <v>86</v>
       </c>
-      <c r="CS1" s="0" t="s">
+      <c r="CS1" t="s">
         <v>87</v>
       </c>
-      <c r="CT1" s="0" t="s">
+      <c r="CT1" t="s">
         <v>52</v>
       </c>
-      <c r="CU1" s="0" t="s">
+      <c r="CU1" t="s">
         <v>88</v>
       </c>
-      <c r="CV1" s="0" t="s">
+      <c r="CV1" t="s">
         <v>10</v>
       </c>
-      <c r="CW1" s="0" t="s">
+      <c r="CW1" t="s">
         <v>11</v>
       </c>
-      <c r="CX1" s="0" t="s">
+      <c r="CX1" t="s">
         <v>12</v>
       </c>
-      <c r="CY1" s="0" t="s">
+      <c r="CY1" t="s">
         <v>13</v>
       </c>
-      <c r="CZ1" s="0" t="s">
+      <c r="CZ1" t="s">
         <v>54</v>
       </c>
-      <c r="DA1" s="0" t="s">
+      <c r="DA1" t="s">
         <v>89</v>
       </c>
-      <c r="DB1" s="0" t="s">
+      <c r="DB1" t="s">
         <v>58</v>
       </c>
-      <c r="DC1" s="0" t="s">
+      <c r="DC1" t="s">
         <v>90</v>
       </c>
-      <c r="DD1" s="0" t="s">
+      <c r="DD1" t="s">
         <v>91</v>
       </c>
-      <c r="DE1" s="0" t="s">
+      <c r="DE1" t="s">
         <v>92</v>
       </c>
-      <c r="DF1" s="0" t="s">
+      <c r="DF1" t="s">
         <v>93</v>
       </c>
-      <c r="DG1" s="0" t="s">
+      <c r="DG1" t="s">
         <v>94</v>
       </c>
-      <c r="DH1" s="0" t="s">
+      <c r="DH1" t="s">
         <v>95</v>
       </c>
-      <c r="DI1" s="0" t="s">
+      <c r="DI1" t="s">
         <v>96</v>
       </c>
-      <c r="DJ1" s="0" t="s">
+      <c r="DJ1" t="s">
         <v>97</v>
       </c>
-      <c r="DK1" s="0" t="s">
+      <c r="DK1" t="s">
         <v>98</v>
       </c>
-      <c r="DL1" s="0" t="s">
+      <c r="DL1" t="s">
         <v>99</v>
       </c>
-      <c r="DM1" s="0" t="s">
+      <c r="DM1" t="s">
         <v>100</v>
       </c>
-      <c r="DN1" s="0" t="s">
+      <c r="DN1" t="s">
         <v>101</v>
       </c>
-      <c r="DO1" s="0" t="s">
+      <c r="DO1" t="s">
         <v>102</v>
       </c>
       <c r="DP1" s="1" t="s">
@@ -1567,115 +2077,115 @@
       <c r="DV1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="DW1" s="0" t="s">
+      <c r="DW1" t="s">
         <v>110</v>
       </c>
-      <c r="DX1" s="0" t="s">
+      <c r="DX1" t="s">
         <v>111</v>
       </c>
-      <c r="DY1" s="0" t="s">
+      <c r="DY1" t="s">
         <v>112</v>
       </c>
-      <c r="DZ1" s="0" t="s">
+      <c r="DZ1" t="s">
         <v>113</v>
       </c>
-      <c r="EA1" s="0" t="s">
+      <c r="EA1" t="s">
         <v>114</v>
       </c>
-      <c r="EB1" s="0" t="s">
+      <c r="EB1" t="s">
         <v>115</v>
       </c>
-      <c r="EC1" s="0" t="s">
+      <c r="EC1" t="s">
         <v>116</v>
       </c>
-      <c r="ED1" s="0" t="s">
+      <c r="ED1" t="s">
         <v>117</v>
       </c>
-      <c r="EE1" s="0" t="s">
+      <c r="EE1" t="s">
         <v>118</v>
       </c>
-      <c r="EF1" s="0" t="s">
+      <c r="EF1" t="s">
         <v>119</v>
       </c>
-      <c r="EG1" s="0" t="s">
+      <c r="EG1" t="s">
         <v>120</v>
       </c>
-      <c r="EH1" s="0" t="s">
+      <c r="EH1" t="s">
         <v>44</v>
       </c>
-      <c r="EI1" s="0" t="s">
+      <c r="EI1" t="s">
         <v>45</v>
       </c>
-      <c r="EJ1" s="0" t="s">
+      <c r="EJ1" t="s">
         <v>121</v>
       </c>
-      <c r="EK1" s="0" t="s">
+      <c r="EK1" t="s">
         <v>122</v>
       </c>
-      <c r="EL1" s="0" t="s">
+      <c r="EL1" t="s">
         <v>123</v>
       </c>
-      <c r="EM1" s="0" t="s">
+      <c r="EM1" t="s">
         <v>124</v>
       </c>
-      <c r="EN1" s="0" t="s">
+      <c r="EN1" t="s">
         <v>125</v>
       </c>
-      <c r="EO1" s="0" t="s">
+      <c r="EO1" t="s">
         <v>46</v>
       </c>
-      <c r="EP1" s="0" t="s">
+      <c r="EP1" t="s">
         <v>49</v>
       </c>
-      <c r="EQ1" s="0" t="s">
+      <c r="EQ1" t="s">
         <v>47</v>
       </c>
-      <c r="ER1" s="0" t="s">
+      <c r="ER1" t="s">
         <v>48</v>
       </c>
-      <c r="ES1" s="0" t="s">
+      <c r="ES1" t="s">
         <v>126</v>
       </c>
-      <c r="ET1" s="0" t="s">
+      <c r="ET1" t="s">
         <v>127</v>
       </c>
-      <c r="EU1" s="0" t="s">
+      <c r="EU1" t="s">
         <v>128</v>
       </c>
-      <c r="EV1" s="0" t="s">
+      <c r="EV1" t="s">
         <v>129</v>
       </c>
-      <c r="EW1" s="0" t="s">
+      <c r="EW1" t="s">
         <v>52</v>
       </c>
-      <c r="EX1" s="0" t="s">
+      <c r="EX1" t="s">
         <v>130</v>
       </c>
-      <c r="EY1" s="0" t="s">
+      <c r="EY1" t="s">
         <v>131</v>
       </c>
-      <c r="EZ1" s="0" t="s">
+      <c r="EZ1" t="s">
         <v>132</v>
       </c>
-      <c r="FA1" s="0" t="s">
+      <c r="FA1" t="s">
         <v>133</v>
       </c>
-      <c r="FB1" s="0" t="s">
+      <c r="FB1" t="s">
         <v>134</v>
       </c>
-      <c r="FC1" s="0" t="s">
+      <c r="FC1" t="s">
         <v>135</v>
       </c>
-      <c r="FD1" s="0" t="s">
+      <c r="FD1" t="s">
         <v>136</v>
       </c>
-      <c r="FE1" s="0" t="s">
+      <c r="FE1" t="s">
         <v>137</v>
       </c>
-      <c r="FF1" s="0" t="s">
+      <c r="FF1" t="s">
         <v>138</v>
       </c>
-      <c r="FG1" s="0" t="s">
+      <c r="FG1" t="s">
         <v>139</v>
       </c>
       <c r="FH1" s="1" t="s">
@@ -1799,9 +2309,9 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
-        <v>42776.3827280324</v>
+    <row r="2" spans="1:203" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>42776.382728032397</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>166</v>
@@ -2081,9 +2591,9 @@
       <c r="GT2" s="1"/>
       <c r="GU2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
-        <v>42776.4220309954</v>
+    <row r="3" spans="1:203" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>42776.422030995403</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>183</v>
@@ -2195,9 +2705,9 @@
       <c r="GT3" s="1"/>
       <c r="GU3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
-        <v>42777.5194228241</v>
+    <row r="4" spans="1:203" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>42777.519422824102</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>190</v>
@@ -2230,9 +2740,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
-        <v>42787.7529152894</v>
+    <row r="5" spans="1:203" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>42787.752915289399</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>196</v>
@@ -2280,9 +2790,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
-        <v>42787.7701543982</v>
+    <row r="6" spans="1:203" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>42787.770154398197</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>201</v>
@@ -2327,8 +2837,8 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+    <row r="7" spans="1:203" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>42787.7937840046</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2387,9 +2897,9 @@
         <v>211</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
-        <v>42788.2231990046</v>
+    <row r="8" spans="1:203" ht="69" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>42788.223199004598</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>212</v>
@@ -2422,9 +2932,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
-        <v>42788.2852648032</v>
+    <row r="9" spans="1:203" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>42788.285264803199</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>215</v>
@@ -2475,9 +2985,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
-        <v>42788.3053630671</v>
+    <row r="10" spans="1:203" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>42788.305363067098</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>218</v>
@@ -2539,13 +3049,13 @@
       <c r="FM10" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="FR10" s="1" t="n">
+      <c r="FR10" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
-        <v>42794.3502083102</v>
+    <row r="11" spans="1:203" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>42794.350208310199</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>224</v>
@@ -2586,16 +3096,16 @@
       <c r="FH11" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="FR11" s="1" t="n">
+      <c r="FR11" s="1">
         <v>1</v>
       </c>
       <c r="FX11" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
-        <v>42794.3659430903</v>
+    <row r="12" spans="1:203" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>42794.365943090299</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>232</v>
@@ -2645,16 +3155,16 @@
       <c r="FH12" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="FR12" s="1" t="n">
+      <c r="FR12" s="1">
         <v>1</v>
       </c>
       <c r="FX12" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="n">
-        <v>42794.4060844097</v>
+    <row r="13" spans="1:203" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>42794.406084409697</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>239</v>
@@ -2704,16 +3214,16 @@
       <c r="FH13" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="FR13" s="1" t="n">
+      <c r="FR13" s="1">
         <v>1</v>
       </c>
       <c r="FX13" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="n">
-        <v>42794.425548912</v>
+    <row r="14" spans="1:203" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>42794.425548911997</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>246</v>
@@ -2773,9 +3283,9 @@
         <v>231</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="n">
-        <v>42795.4736184491</v>
+    <row r="15" spans="1:203" ht="193.2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>42795.473618449098</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>251</v>
@@ -2847,9 +3357,9 @@
         <v>231</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="n">
-        <v>42795.8458275579</v>
+    <row r="16" spans="1:203" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>42795.845827557903</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>258</v>
@@ -2978,9 +3488,9 @@
         <v>231</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="n">
-        <v>42795.8982552893</v>
+    <row r="17" spans="1:191" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>42795.898255289299</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>264</v>
@@ -3055,9 +3565,9 @@
         <v>231</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="n">
-        <v>42795.9227740972</v>
+    <row r="18" spans="1:191" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>42795.922774097198</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>269</v>
@@ -3146,7 +3656,7 @@
       <c r="FN18" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="FR18" s="1" t="n">
+      <c r="FR18" s="1">
         <v>3</v>
       </c>
       <c r="FX18" s="1" t="s">
@@ -3165,9 +3675,9 @@
       <c r="GH18" s="1"/>
       <c r="GI18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="n">
-        <v>42796.1386970023</v>
+    <row r="19" spans="1:191" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>42796.138697002301</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>278</v>
@@ -3223,16 +3733,16 @@
       <c r="FH19" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="FR19" s="1" t="n">
+      <c r="FR19" s="1">
         <v>1</v>
       </c>
       <c r="FX19" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="n">
-        <v>42796.6060339005</v>
+    <row r="20" spans="1:191" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>42796.606033900498</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>282</v>
@@ -3316,8 +3826,8 @@
       <c r="GH20" s="1"/>
       <c r="GI20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="n">
+    <row r="21" spans="1:191" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>42796.7542410764</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -3396,9 +3906,9 @@
       <c r="GH21" s="1"/>
       <c r="GI21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="n">
-        <v>42797.5396422222</v>
+    <row r="22" spans="1:191" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>42797.539642222197</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>295</v>
@@ -3473,9 +3983,9 @@
       <c r="GH22" s="1"/>
       <c r="GI22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="n">
-        <v>42797.7591014699</v>
+    <row r="23" spans="1:191" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>42797.759101469899</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>301</v>
@@ -3541,8 +4051,8 @@
         <v>231</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="n">
+    <row r="24" spans="1:191" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>42797.7796537963</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -3621,9 +4131,9 @@
         <v>231</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="n">
-        <v>42797.7907061343</v>
+    <row r="25" spans="1:191" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>42797.790706134299</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>308</v>
@@ -3731,22 +4241,17 @@
         <v>231</v>
       </c>
     </row>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1048570" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1048571" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1048572" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>